<commit_message>
Task Enumartaion Spreadsheet Updated
</commit_message>
<xml_diff>
--- a/Petros/Task Enumeration.xlsx
+++ b/Petros/Task Enumeration.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FAST BACKUP_DESKTOP\Career Related\Career Enhancement\Engineering Accelarator\Fall-2017\Petros\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -75,7 +80,34 @@
     <t xml:space="preserve">Test </t>
   </si>
   <si>
-    <t xml:space="preserve">Flow Diagram </t>
+    <t>Featuere Diagram</t>
+  </si>
+  <si>
+    <t>Familirizing inkscape</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Preparing version one</t>
+  </si>
+  <si>
+    <t>Revisualizing the whole project</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Feature diagram vesion 2</t>
+  </si>
+  <si>
+    <t>Refering to similar format</t>
+  </si>
+  <si>
+    <t>Preparing version 1 on Notepad++</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
   </si>
 </sst>
 </file>
@@ -169,6 +201,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -497,16 +537,16 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +558,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="16">
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -530,7 +570,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:11" ht="16">
+    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -540,7 +580,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="16">
+    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -575,35 +615,131 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>3.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>

</xml_diff>